<commit_message>
Reimbursement unit related tests completed
</commit_message>
<xml_diff>
--- a/reimbursement/src/main/resources/TestData/ReimbUnits/ReimbUnitsCreationScenarios.xlsx
+++ b/reimbursement/src/main/resources/TestData/ReimbUnits/ReimbUnitsCreationScenarios.xlsx
@@ -195,13 +195,13 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.32"/>

</xml_diff>

<commit_message>
//Reimb Form Object classes
</commit_message>
<xml_diff>
--- a/reimbursement/src/main/resources/TestData/ReimbUnits/ReimbUnitsCreationScenarios.xlsx
+++ b/reimbursement/src/main/resources/TestData/ReimbUnits/ReimbUnitsCreationScenarios.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -46,22 +46,10 @@
     <t xml:space="preserve">AutoUnit1</t>
   </si>
   <si>
-    <t xml:space="preserve">Create Custom flow1</t>
+    <t xml:space="preserve">Create Reimbursement flow1</t>
   </si>
   <si>
     <t xml:space="preserve">AutoUnit1_Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reimb Unit Form auto2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AutoUnit2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create Custom flow2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AutoUnit2_Description</t>
   </si>
 </sst>
 </file>
@@ -71,7 +59,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -106,12 +94,6 @@
       <b val="true"/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -158,7 +140,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -168,10 +150,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -195,7 +173,7 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -231,33 +209,17 @@
       <c r="B2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="0" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>